<commit_message>
found problems with dataset
</commit_message>
<xml_diff>
--- a/File_Excel/commenti_hS_per_topic.xlsx
+++ b/File_Excel/commenti_hS_per_topic.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -485,7 +485,7 @@
       <c r="A3" t="inlineStr"/>
       <c r="B3" t="inlineStr">
         <is>
-          <t>CRONACA</t>
+          <t>CROANCA</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -494,16 +494,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E3" t="n">
-        <v>1166</v>
+        <v>33</v>
       </c>
       <c r="F3" t="n">
-        <v>80</v>
+        <v>3</v>
       </c>
       <c r="G3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -515,20 +515,20 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Instagram</t>
+          <t>Facebook</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E4" t="n">
-        <v>908</v>
+        <v>1058</v>
       </c>
       <c r="F4" t="n">
-        <v>177</v>
+        <v>81</v>
       </c>
       <c r="G4" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
@@ -540,45 +540,45 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>YouTube</t>
+          <t>Instagram</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E5" t="n">
-        <v>1046</v>
+        <v>939</v>
       </c>
       <c r="F5" t="n">
-        <v>74</v>
+        <v>174</v>
       </c>
       <c r="G5" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr"/>
       <c r="B6" t="inlineStr">
         <is>
-          <t>CRONACA NERA</t>
+          <t>CRONACA</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Facebook</t>
+          <t>YouTube</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="E6" t="n">
-        <v>892</v>
+        <v>1093</v>
       </c>
       <c r="F6" t="n">
-        <v>136</v>
+        <v>77</v>
       </c>
       <c r="G6" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7">
@@ -590,20 +590,20 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Instagram</t>
+          <t>Facebook</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E7" t="n">
-        <v>829</v>
+        <v>1014</v>
       </c>
       <c r="F7" t="n">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="G7" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8">
@@ -615,42 +615,42 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>YouTube</t>
+          <t>Instagram</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="E8" t="n">
-        <v>1046</v>
+        <v>996</v>
       </c>
       <c r="F8" t="n">
-        <v>62</v>
+        <v>168</v>
       </c>
       <c r="G8" t="n">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr"/>
       <c r="B9" t="inlineStr">
         <is>
-          <t>POLITICA</t>
+          <t>CRONACA NERA</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Facebook</t>
+          <t>YouTube</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E9" t="n">
-        <v>1037</v>
+        <v>1117</v>
       </c>
       <c r="F9" t="n">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="G9" t="n">
         <v>5</v>
@@ -665,20 +665,20 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Instagram</t>
+          <t>Facebook</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="E10" t="n">
-        <v>936</v>
+        <v>1111</v>
       </c>
       <c r="F10" t="n">
-        <v>142</v>
+        <v>69</v>
       </c>
       <c r="G10" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11">
@@ -690,19 +690,44 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>38</v>
+      </c>
+      <c r="E11" t="n">
+        <v>1001</v>
+      </c>
+      <c r="F11" t="n">
+        <v>145</v>
+      </c>
+      <c r="G11" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr"/>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>POLITICA</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
           <t>YouTube</t>
         </is>
       </c>
-      <c r="D11" t="n">
-        <v>22</v>
-      </c>
-      <c r="E11" t="n">
-        <v>995</v>
-      </c>
-      <c r="F11" t="n">
-        <v>59</v>
-      </c>
-      <c r="G11" t="n">
+      <c r="D12" t="n">
+        <v>21</v>
+      </c>
+      <c r="E12" t="n">
+        <v>1104</v>
+      </c>
+      <c r="F12" t="n">
+        <v>68</v>
+      </c>
+      <c r="G12" t="n">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added rows to dataset and added pies
</commit_message>
<xml_diff>
--- a/File_Excel/commenti_hS_per_topic.xlsx
+++ b/File_Excel/commenti_hS_per_topic.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -485,7 +485,7 @@
       <c r="A3" t="inlineStr"/>
       <c r="B3" t="inlineStr">
         <is>
-          <t>CROANCA</t>
+          <t>CRONACA</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -494,16 +494,16 @@
         </is>
       </c>
       <c r="D3" t="n">
+        <v>15</v>
+      </c>
+      <c r="E3" t="n">
+        <v>1093</v>
+      </c>
+      <c r="F3" t="n">
+        <v>85</v>
+      </c>
+      <c r="G3" t="n">
         <v>3</v>
-      </c>
-      <c r="E3" t="n">
-        <v>33</v>
-      </c>
-      <c r="F3" t="n">
-        <v>3</v>
-      </c>
-      <c r="G3" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -515,20 +515,20 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Facebook</t>
+          <t>Instagram</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E4" t="n">
-        <v>1058</v>
+        <v>995</v>
       </c>
       <c r="F4" t="n">
-        <v>81</v>
+        <v>181</v>
       </c>
       <c r="G4" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5">
@@ -540,45 +540,45 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Instagram</t>
+          <t>YouTube</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="E5" t="n">
-        <v>939</v>
+        <v>1101</v>
       </c>
       <c r="F5" t="n">
-        <v>174</v>
+        <v>77</v>
       </c>
       <c r="G5" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr"/>
       <c r="B6" t="inlineStr">
         <is>
-          <t>CRONACA</t>
+          <t>CRONACA NERA</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>YouTube</t>
+          <t>Facebook</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="E6" t="n">
-        <v>1093</v>
+        <v>1014</v>
       </c>
       <c r="F6" t="n">
-        <v>77</v>
+        <v>150</v>
       </c>
       <c r="G6" t="n">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7">
@@ -590,20 +590,20 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Facebook</t>
+          <t>Instagram</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E7" t="n">
-        <v>1014</v>
+        <v>996</v>
       </c>
       <c r="F7" t="n">
-        <v>150</v>
+        <v>168</v>
       </c>
       <c r="G7" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8">
@@ -615,42 +615,42 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Instagram</t>
+          <t>YouTube</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="E8" t="n">
-        <v>996</v>
+        <v>1117</v>
       </c>
       <c r="F8" t="n">
-        <v>168</v>
+        <v>66</v>
       </c>
       <c r="G8" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr"/>
       <c r="B9" t="inlineStr">
         <is>
-          <t>CRONACA NERA</t>
+          <t>POLITICA</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>YouTube</t>
+          <t>Facebook</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E9" t="n">
-        <v>1117</v>
+        <v>1111</v>
       </c>
       <c r="F9" t="n">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="G9" t="n">
         <v>5</v>
@@ -665,20 +665,20 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Facebook</t>
+          <t>Instagram</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="E10" t="n">
-        <v>1111</v>
+        <v>1008</v>
       </c>
       <c r="F10" t="n">
-        <v>69</v>
+        <v>145</v>
       </c>
       <c r="G10" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11">
@@ -690,44 +690,19 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Instagram</t>
+          <t>YouTube</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="E11" t="n">
-        <v>1001</v>
+        <v>1104</v>
       </c>
       <c r="F11" t="n">
-        <v>145</v>
+        <v>68</v>
       </c>
       <c r="G11" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr"/>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>POLITICA</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>YouTube</t>
-        </is>
-      </c>
-      <c r="D12" t="n">
-        <v>21</v>
-      </c>
-      <c r="E12" t="n">
-        <v>1104</v>
-      </c>
-      <c r="F12" t="n">
-        <v>68</v>
-      </c>
-      <c r="G12" t="n">
         <v>2</v>
       </c>
     </row>

</xml_diff>